<commit_message>
i want to update xlsx_file need to study code
</commit_message>
<xml_diff>
--- a/my_book.xlsx
+++ b/my_book.xlsx
@@ -493,7 +493,7 @@
         </is>
       </c>
       <c r="G4" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="G5" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -569,7 +569,7 @@
         </is>
       </c>
       <c r="G6" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="G7" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -645,7 +645,7 @@
         </is>
       </c>
       <c r="G8" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -683,7 +683,7 @@
         </is>
       </c>
       <c r="G9" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="G10" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -759,7 +759,7 @@
         </is>
       </c>
       <c r="G11" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="G12" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -835,7 +835,7 @@
         </is>
       </c>
       <c r="G13" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -873,7 +873,7 @@
         </is>
       </c>
       <c r="G14" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -911,7 +911,7 @@
         </is>
       </c>
       <c r="G15" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="G16" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -987,7 +987,7 @@
         </is>
       </c>
       <c r="G17" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="G18" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="G19" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1101,7 +1101,7 @@
         </is>
       </c>
       <c r="G20" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1139,7 +1139,7 @@
         </is>
       </c>
       <c r="G21" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1177,7 +1177,7 @@
         </is>
       </c>
       <c r="G22" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -1215,7 +1215,7 @@
         </is>
       </c>
       <c r="G23" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1253,7 +1253,7 @@
         </is>
       </c>
       <c r="G24" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1291,7 +1291,7 @@
         </is>
       </c>
       <c r="G25" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -1329,7 +1329,7 @@
         </is>
       </c>
       <c r="G26" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
@@ -1367,7 +1367,7 @@
         </is>
       </c>
       <c r="G27" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         </is>
       </c>
       <c r="G28" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -1443,7 +1443,7 @@
         </is>
       </c>
       <c r="G29" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -1481,7 +1481,7 @@
         </is>
       </c>
       <c r="G30" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
@@ -1519,7 +1519,7 @@
         </is>
       </c>
       <c r="G31" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -1557,7 +1557,7 @@
         </is>
       </c>
       <c r="G32" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -1595,7 +1595,7 @@
         </is>
       </c>
       <c r="G33" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
@@ -1633,7 +1633,7 @@
         </is>
       </c>
       <c r="G34" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
@@ -1671,7 +1671,7 @@
         </is>
       </c>
       <c r="G35" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -1709,7 +1709,7 @@
         </is>
       </c>
       <c r="G36" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
@@ -1747,7 +1747,7 @@
         </is>
       </c>
       <c r="G37" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
@@ -1785,7 +1785,7 @@
         </is>
       </c>
       <c r="G38" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
@@ -1823,7 +1823,7 @@
         </is>
       </c>
       <c r="G39" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
@@ -1861,7 +1861,7 @@
         </is>
       </c>
       <c r="G40" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
@@ -1899,7 +1899,7 @@
         </is>
       </c>
       <c r="G41" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
@@ -1937,7 +1937,7 @@
         </is>
       </c>
       <c r="G42" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
@@ -1975,7 +1975,7 @@
         </is>
       </c>
       <c r="G43" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -2013,7 +2013,7 @@
         </is>
       </c>
       <c r="G44" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
@@ -2051,7 +2051,7 @@
         </is>
       </c>
       <c r="G45" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
@@ -2089,7 +2089,7 @@
         </is>
       </c>
       <c r="G46" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
@@ -2127,7 +2127,7 @@
         </is>
       </c>
       <c r="G47" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
@@ -2165,7 +2165,7 @@
         </is>
       </c>
       <c r="G48" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
@@ -2203,7 +2203,7 @@
         </is>
       </c>
       <c r="G49" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
@@ -2241,7 +2241,7 @@
         </is>
       </c>
       <c r="G50" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
@@ -2279,7 +2279,7 @@
         </is>
       </c>
       <c r="G51" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
@@ -2317,7 +2317,7 @@
         </is>
       </c>
       <c r="G52" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
@@ -2355,7 +2355,7 @@
         </is>
       </c>
       <c r="G53" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
@@ -2393,7 +2393,7 @@
         </is>
       </c>
       <c r="G54" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
@@ -2431,7 +2431,7 @@
         </is>
       </c>
       <c r="G55" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
@@ -2469,7 +2469,7 @@
         </is>
       </c>
       <c r="G56" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
@@ -2507,7 +2507,7 @@
         </is>
       </c>
       <c r="G57" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
@@ -2545,7 +2545,7 @@
         </is>
       </c>
       <c r="G58" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
@@ -2583,7 +2583,7 @@
         </is>
       </c>
       <c r="G59" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
@@ -2621,7 +2621,7 @@
         </is>
       </c>
       <c r="G60" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
@@ -2659,7 +2659,7 @@
         </is>
       </c>
       <c r="G61" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
@@ -2697,7 +2697,7 @@
         </is>
       </c>
       <c r="G62" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
@@ -2735,7 +2735,7 @@
         </is>
       </c>
       <c r="G63" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
@@ -2773,7 +2773,7 @@
         </is>
       </c>
       <c r="G64" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
@@ -2811,7 +2811,7 @@
         </is>
       </c>
       <c r="G65" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
@@ -2849,7 +2849,7 @@
         </is>
       </c>
       <c r="G66" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
@@ -2887,7 +2887,7 @@
         </is>
       </c>
       <c r="G67" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
@@ -2925,7 +2925,7 @@
         </is>
       </c>
       <c r="G68" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H68" t="inlineStr">
         <is>
@@ -2963,7 +2963,7 @@
         </is>
       </c>
       <c r="G69" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="G70" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
@@ -3039,7 +3039,7 @@
         </is>
       </c>
       <c r="G71" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
@@ -3077,7 +3077,7 @@
         </is>
       </c>
       <c r="G72" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
@@ -3115,7 +3115,7 @@
         </is>
       </c>
       <c r="G73" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
         </is>
       </c>
       <c r="G74" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
@@ -3191,7 +3191,7 @@
         </is>
       </c>
       <c r="G75" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H75" t="inlineStr">
         <is>
@@ -3229,7 +3229,7 @@
         </is>
       </c>
       <c r="G76" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H76" t="inlineStr">
         <is>
@@ -3267,7 +3267,7 @@
         </is>
       </c>
       <c r="G77" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H77" t="inlineStr">
         <is>
@@ -3305,7 +3305,7 @@
         </is>
       </c>
       <c r="G78" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H78" t="inlineStr">
         <is>
@@ -3343,7 +3343,7 @@
         </is>
       </c>
       <c r="G79" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H79" t="inlineStr">
         <is>
@@ -3381,7 +3381,7 @@
         </is>
       </c>
       <c r="G80" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
@@ -3419,7 +3419,7 @@
         </is>
       </c>
       <c r="G81" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
@@ -3457,7 +3457,7 @@
         </is>
       </c>
       <c r="G82" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
@@ -3495,7 +3495,7 @@
         </is>
       </c>
       <c r="G83" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
@@ -3533,7 +3533,7 @@
         </is>
       </c>
       <c r="G84" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
@@ -3571,7 +3571,7 @@
         </is>
       </c>
       <c r="G85" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
@@ -3609,7 +3609,7 @@
         </is>
       </c>
       <c r="G86" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H86" t="inlineStr">
         <is>
@@ -3647,7 +3647,7 @@
         </is>
       </c>
       <c r="G87" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H87" t="inlineStr">
         <is>
@@ -3685,7 +3685,7 @@
         </is>
       </c>
       <c r="G88" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H88" t="inlineStr">
         <is>
@@ -3723,7 +3723,7 @@
         </is>
       </c>
       <c r="G89" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H89" t="inlineStr">
         <is>
@@ -3761,7 +3761,7 @@
         </is>
       </c>
       <c r="G90" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H90" t="inlineStr">
         <is>
@@ -3799,7 +3799,7 @@
         </is>
       </c>
       <c r="G91" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H91" t="inlineStr">
         <is>
@@ -3837,7 +3837,7 @@
         </is>
       </c>
       <c r="G92" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H92" t="inlineStr">
         <is>
@@ -3875,7 +3875,7 @@
         </is>
       </c>
       <c r="G93" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H93" t="inlineStr">
         <is>
@@ -3913,7 +3913,7 @@
         </is>
       </c>
       <c r="G94" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H94" t="inlineStr">
         <is>
@@ -3951,7 +3951,7 @@
         </is>
       </c>
       <c r="G95" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H95" t="inlineStr">
         <is>
@@ -3989,7 +3989,7 @@
         </is>
       </c>
       <c r="G96" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
@@ -4027,7 +4027,7 @@
         </is>
       </c>
       <c r="G97" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
@@ -4065,7 +4065,7 @@
         </is>
       </c>
       <c r="G98" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H98" t="inlineStr">
         <is>
@@ -4103,7 +4103,7 @@
         </is>
       </c>
       <c r="G99" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
@@ -4141,7 +4141,7 @@
         </is>
       </c>
       <c r="G100" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H100" t="inlineStr">
         <is>
@@ -4179,7 +4179,7 @@
         </is>
       </c>
       <c r="G101" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H101" t="inlineStr">
         <is>
@@ -4217,7 +4217,7 @@
         </is>
       </c>
       <c r="G102" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H102" t="inlineStr">
         <is>
@@ -4255,7 +4255,7 @@
         </is>
       </c>
       <c r="G103" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H103" t="inlineStr">
         <is>
@@ -4293,7 +4293,7 @@
         </is>
       </c>
       <c r="G104" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
@@ -4331,7 +4331,7 @@
         </is>
       </c>
       <c r="G105" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H105" t="inlineStr">
         <is>
@@ -4369,7 +4369,7 @@
         </is>
       </c>
       <c r="G106" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H106" t="inlineStr">
         <is>
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="G107" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H107" t="inlineStr">
         <is>
@@ -4445,7 +4445,7 @@
         </is>
       </c>
       <c r="G108" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H108" t="inlineStr">
         <is>
@@ -4483,7 +4483,7 @@
         </is>
       </c>
       <c r="G109" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H109" t="inlineStr">
         <is>
@@ -4521,7 +4521,7 @@
         </is>
       </c>
       <c r="G110" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H110" t="inlineStr">
         <is>
@@ -4559,7 +4559,7 @@
         </is>
       </c>
       <c r="G111" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H111" t="inlineStr">
         <is>
@@ -4597,7 +4597,7 @@
         </is>
       </c>
       <c r="G112" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H112" t="inlineStr">
         <is>
@@ -4635,7 +4635,7 @@
         </is>
       </c>
       <c r="G113" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H113" t="inlineStr">
         <is>
@@ -4673,7 +4673,7 @@
         </is>
       </c>
       <c r="G114" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H114" t="inlineStr">
         <is>
@@ -4711,7 +4711,7 @@
         </is>
       </c>
       <c r="G115" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H115" t="inlineStr">
         <is>
@@ -4749,7 +4749,7 @@
         </is>
       </c>
       <c r="G116" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H116" t="inlineStr">
         <is>
@@ -4787,7 +4787,7 @@
         </is>
       </c>
       <c r="G117" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H117" t="inlineStr">
         <is>
@@ -4825,7 +4825,7 @@
         </is>
       </c>
       <c r="G118" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H118" t="inlineStr">
         <is>
@@ -4863,7 +4863,7 @@
         </is>
       </c>
       <c r="G119" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H119" t="inlineStr">
         <is>
@@ -4901,7 +4901,7 @@
         </is>
       </c>
       <c r="G120" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H120" t="inlineStr">
         <is>
@@ -4939,7 +4939,7 @@
         </is>
       </c>
       <c r="G121" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H121" t="inlineStr">
         <is>
@@ -4977,7 +4977,7 @@
         </is>
       </c>
       <c r="G122" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H122" t="inlineStr">
         <is>
@@ -5015,7 +5015,7 @@
         </is>
       </c>
       <c r="G123" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H123" t="inlineStr">
         <is>
@@ -5053,7 +5053,7 @@
         </is>
       </c>
       <c r="G124" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H124" t="inlineStr">
         <is>
@@ -5091,7 +5091,7 @@
         </is>
       </c>
       <c r="G125" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H125" t="inlineStr">
         <is>
@@ -5129,7 +5129,7 @@
         </is>
       </c>
       <c r="G126" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H126" t="inlineStr">
         <is>
@@ -5167,7 +5167,7 @@
         </is>
       </c>
       <c r="G127" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H127" t="inlineStr">
         <is>
@@ -5205,7 +5205,7 @@
         </is>
       </c>
       <c r="G128" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H128" t="inlineStr">
         <is>
@@ -5243,7 +5243,7 @@
         </is>
       </c>
       <c r="G129" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H129" t="inlineStr">
         <is>
@@ -5281,7 +5281,7 @@
         </is>
       </c>
       <c r="G130" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H130" t="inlineStr">
         <is>
@@ -5319,7 +5319,7 @@
         </is>
       </c>
       <c r="G131" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H131" t="inlineStr">
         <is>
@@ -5357,7 +5357,7 @@
         </is>
       </c>
       <c r="G132" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H132" t="inlineStr">
         <is>
@@ -5395,7 +5395,7 @@
         </is>
       </c>
       <c r="G133" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H133" t="inlineStr">
         <is>
@@ -5433,7 +5433,7 @@
         </is>
       </c>
       <c r="G134" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H134" t="inlineStr">
         <is>
@@ -5471,7 +5471,7 @@
         </is>
       </c>
       <c r="G135" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H135" t="inlineStr">
         <is>
@@ -5509,7 +5509,7 @@
         </is>
       </c>
       <c r="G136" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H136" t="inlineStr">
         <is>
@@ -5547,7 +5547,7 @@
         </is>
       </c>
       <c r="G137" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H137" t="inlineStr">
         <is>
@@ -5585,7 +5585,7 @@
         </is>
       </c>
       <c r="G138" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H138" t="inlineStr">
         <is>
@@ -5623,7 +5623,7 @@
         </is>
       </c>
       <c r="G139" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H139" t="inlineStr">
         <is>
@@ -5661,7 +5661,7 @@
         </is>
       </c>
       <c r="G140" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H140" t="inlineStr">
         <is>
@@ -5699,7 +5699,7 @@
         </is>
       </c>
       <c r="G141" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H141" t="inlineStr">
         <is>
@@ -5737,7 +5737,7 @@
         </is>
       </c>
       <c r="G142" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H142" t="inlineStr">
         <is>
@@ -5775,7 +5775,7 @@
         </is>
       </c>
       <c r="G143" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H143" t="inlineStr">
         <is>
@@ -5813,7 +5813,7 @@
         </is>
       </c>
       <c r="G144" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H144" t="inlineStr">
         <is>
@@ -5851,7 +5851,7 @@
         </is>
       </c>
       <c r="G145" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H145" t="inlineStr">
         <is>
@@ -5889,7 +5889,7 @@
         </is>
       </c>
       <c r="G146" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H146" t="inlineStr">
         <is>
@@ -5927,7 +5927,7 @@
         </is>
       </c>
       <c r="G147" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H147" t="inlineStr">
         <is>
@@ -5965,7 +5965,7 @@
         </is>
       </c>
       <c r="G148" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H148" t="inlineStr">
         <is>
@@ -6003,7 +6003,7 @@
         </is>
       </c>
       <c r="G149" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H149" t="inlineStr">
         <is>
@@ -6041,7 +6041,7 @@
         </is>
       </c>
       <c r="G150" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H150" t="inlineStr">
         <is>
@@ -6079,7 +6079,7 @@
         </is>
       </c>
       <c r="G151" s="1" t="n">
-        <v>45498</v>
+        <v>45505</v>
       </c>
       <c r="H151" t="inlineStr">
         <is>

</xml_diff>